<commit_message>
Beautiful graphics + duty cicle working
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J799"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1055,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="1">
-        <v>123456789</v>
+        <v>0.123456789</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value entered must be a legal alignment value (e.g. LEFT).">
           <x14:formula1>
             <xm:f>'Internal Values'!$A$2:$A$48</xm:f>

</xml_diff>